<commit_message>
Fix layout using Tailwindcss, commit v3
</commit_message>
<xml_diff>
--- a/SampleXLSX/sample.xlsx
+++ b/SampleXLSX/sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Desktop\traCuuThongTin\SampleXLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B446B2BE-143C-4CB6-8AC3-368066B0B301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA69689-0D11-44C0-B64B-4DB8EB78F821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="72">
   <si>
     <t>SỞ GDĐT HÀ NỘI</t>
   </si>
@@ -225,6 +225,45 @@
   </si>
   <si>
     <t>Nguyễn Khắc Long</t>
+  </si>
+  <si>
+    <t>01167
+ANHU</t>
+  </si>
+  <si>
+    <t>01166
+ANHU</t>
+  </si>
+  <si>
+    <t>01165
+ANHU</t>
+  </si>
+  <si>
+    <t>01164
+ANHU</t>
+  </si>
+  <si>
+    <t>01163
+ANHU</t>
+  </si>
+  <si>
+    <t>01162
+ANHU</t>
+  </si>
+  <si>
+    <t>Nguyễn Trần Tuấn</t>
+  </si>
+  <si>
+    <t>Phạm Thế Tuấn</t>
+  </si>
+  <si>
+    <t>Hào Thế Long</t>
+  </si>
+  <si>
+    <t>Lò Thế Khanh</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Tuấn</t>
   </si>
 </sst>
 </file>
@@ -617,10 +656,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="K7" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1341,8 +1380,449 @@
         <v>42</v>
       </c>
     </row>
+    <row r="13" spans="1:23" ht="33.6">
+      <c r="A13" s="13">
+        <f>IF(B13="","",SUBTOTAL(3,$B$6:$B13))</f>
+        <v>8</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O13" s="14">
+        <v>10</v>
+      </c>
+      <c r="P13" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>30</v>
+      </c>
+      <c r="R13" s="14">
+        <v>30</v>
+      </c>
+      <c r="S13" s="14">
+        <v>50</v>
+      </c>
+      <c r="T13" s="18">
+        <f t="shared" ref="T13:T18" si="2">SUM(O13:S13)</f>
+        <v>140</v>
+      </c>
+      <c r="U13" s="18">
+        <v>10</v>
+      </c>
+      <c r="V13" s="18">
+        <f t="shared" ref="V13:V18" si="3">T13+U13</f>
+        <v>150</v>
+      </c>
+      <c r="W13" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="33.6">
+      <c r="A14" s="13">
+        <f>IF(B14="","",SUBTOTAL(3,$B$6:$B14))</f>
+        <v>9</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O14" s="14">
+        <v>50</v>
+      </c>
+      <c r="P14" s="14">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>30</v>
+      </c>
+      <c r="R14" s="14">
+        <v>30</v>
+      </c>
+      <c r="S14" s="14">
+        <v>50</v>
+      </c>
+      <c r="T14" s="18">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="U14" s="18">
+        <v>10</v>
+      </c>
+      <c r="V14" s="18">
+        <f t="shared" si="3"/>
+        <v>220</v>
+      </c>
+      <c r="W14" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="33.6">
+      <c r="A15" s="13">
+        <f>IF(B15="","",SUBTOTAL(3,$B$6:$B15))</f>
+        <v>10</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="G15" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O15" s="14">
+        <v>10</v>
+      </c>
+      <c r="P15" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>30</v>
+      </c>
+      <c r="R15" s="14">
+        <v>30</v>
+      </c>
+      <c r="S15" s="14">
+        <v>50</v>
+      </c>
+      <c r="T15" s="18">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18">
+        <f t="shared" si="3"/>
+        <v>140</v>
+      </c>
+      <c r="W15" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="33.6">
+      <c r="A16" s="13">
+        <f>IF(B16="","",SUBTOTAL(3,$B$6:$B16))</f>
+        <v>11</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M16" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="14">
+        <v>10</v>
+      </c>
+      <c r="P16" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="14">
+        <v>40</v>
+      </c>
+      <c r="R16" s="14">
+        <v>30</v>
+      </c>
+      <c r="S16" s="14">
+        <v>50</v>
+      </c>
+      <c r="T16" s="18">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18">
+        <f t="shared" si="3"/>
+        <v>150</v>
+      </c>
+      <c r="W16" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="33.6">
+      <c r="A17" s="13">
+        <f>IF(B17="","",SUBTOTAL(3,$B$6:$B17))</f>
+        <v>12</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="14">
+        <v>10</v>
+      </c>
+      <c r="P17" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q17" s="14">
+        <v>30</v>
+      </c>
+      <c r="R17" s="14">
+        <v>50</v>
+      </c>
+      <c r="S17" s="14">
+        <v>50</v>
+      </c>
+      <c r="T17" s="18">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="U17" s="18">
+        <v>10</v>
+      </c>
+      <c r="V17" s="18">
+        <f t="shared" si="3"/>
+        <v>170</v>
+      </c>
+      <c r="W17" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="33.6">
+      <c r="A18" s="13">
+        <f>IF(B18="","",SUBTOTAL(3,$B$6:$B18))</f>
+        <v>13</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="M18" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="14">
+        <v>40</v>
+      </c>
+      <c r="P18" s="14">
+        <v>20</v>
+      </c>
+      <c r="Q18" s="14">
+        <v>30</v>
+      </c>
+      <c r="R18" s="14">
+        <v>30</v>
+      </c>
+      <c r="S18" s="14">
+        <v>50</v>
+      </c>
+      <c r="T18" s="18">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="U18" s="18">
+        <v>10</v>
+      </c>
+      <c r="V18" s="18">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="W18" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:I4"/>
@@ -1359,7 +1839,6 @@
     <mergeCell ref="M4:M5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="O4:V4"/>
-    <mergeCell ref="D4:D5"/>
   </mergeCells>
   <pageMargins left="0.26" right="0.17" top="0.2" bottom="0.24" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>

</xml_diff>